<commit_message>
Modified RPA_Testing/Word Hashing process.
</commit_message>
<xml_diff>
--- a/RPA_Testing/Results.xlsx
+++ b/RPA_Testing/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\68228\Documents\UiPath\RPA_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb877d285e39445/Desktop/UiPath_Practice_Problems/RPA_Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E8C717-139F-4154-B4BE-6062D2FBB835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{36E8C717-139F-4154-B4BE-6062D2FBB835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9563C5B0-A294-4BD1-A8F3-5B99E91A4E0A}"/>
   <x:bookViews>
-    <x:workbookView xWindow="40860" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <x:si>
     <x:t>HashMethod</x:t>
   </x:si>
   <x:si>
-    <x:t>Result</x:t>
+    <x:t>Word Choice</x:t>
   </x:si>
   <x:si>
     <x:t>Web_Result</x:t>
@@ -35,175 +35,118 @@
     <x:t>gost</x:t>
   </x:si>
   <x:si>
-    <x:t>cc54f6b5a095dfc6cb6eb17dcbf8cc15a4f0ca7a154a2724b7226797c9d7457c</x:t>
-  </x:si>
-  <x:si>
-    <x:t>941925baf905c9fc168cac2656ce11a962e294db8d2af664c47b3918fac4a8b6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Match</x:t>
+    <x:t>Elucidate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bca0ac31500f40bdc1000e0aef880e73c817b5600fccf89dda1c198ed0b9e67e</x:t>
   </x:si>
   <x:si>
     <x:t>adler32</x:t>
   </x:si>
   <x:si>
-    <x:t>07c4024c</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0d8c0325</x:t>
+    <x:t>11680391</x:t>
   </x:si>
   <x:si>
     <x:t>crc32</x:t>
   </x:si>
   <x:si>
-    <x:t>44ab5e0d</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ebaa5d53</x:t>
+    <x:t>ad93dfac</x:t>
   </x:si>
   <x:si>
     <x:t>crc32b</x:t>
   </x:si>
   <x:si>
-    <x:t>f381d6f6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ebc82cd9</x:t>
+    <x:t>da809830</x:t>
   </x:si>
   <x:si>
     <x:t>haval128,3</x:t>
   </x:si>
   <x:si>
-    <x:t>6b7b813e06b46d4b2f28185545618062</x:t>
-  </x:si>
-  <x:si>
-    <x:t>d61492f254562f1529dc36af0770ffe9</x:t>
+    <x:t>f8248dd2ec3b670a7a310407d0943c3f</x:t>
   </x:si>
   <x:si>
     <x:t>haval160,3</x:t>
   </x:si>
   <x:si>
-    <x:t>300c5967c3bbd8b1ad580c89ba38c18b2a507fd2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0ec51a6aaadef2e3adc3e0ea1d718c154bda7b74</x:t>
+    <x:t>7c8fc2ccdc68148861edf6549f782d3b2a4f7e0d</x:t>
   </x:si>
   <x:si>
     <x:t>haval192,3</x:t>
   </x:si>
   <x:si>
-    <x:t>f48675616959b4e7f8399a0945c3762a54d0ae890273b211</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0fc6d28ec7237ecedd38c38f0ec124aaedf8f35d6e99b4e0</x:t>
+    <x:t>300bf3138202e8ac8d1c8fc67e40f476d29d01bf34a2f94e</x:t>
   </x:si>
   <x:si>
     <x:t>haval224,3</x:t>
   </x:si>
   <x:si>
-    <x:t>fe7a818f332516d2d25b8307c02544e76ca5522e0c38b47663886548</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f908ad0a74c7e6f086438746a7b0c1252eb7c900f4353c1fdbb4e60b</x:t>
+    <x:t>77b84524ad0ab4fbf82c6e97aca950bb7d89919a5063521aa211267b</x:t>
   </x:si>
   <x:si>
     <x:t>haval256,3</x:t>
   </x:si>
   <x:si>
-    <x:t>ed6fc4ecbec7b3ea54d54a0108eaa5b2bddfae599844371987b21b26016ad325</x:t>
-  </x:si>
-  <x:si>
-    <x:t>f58f14bf9ff82fa05eba49856d26304f30a455e8e0edb8eb764efadabca1af90</x:t>
+    <x:t>05740fa99fbd750d66dc32b4c9076d1aff28c927ed3f17533aff918b5d899c91</x:t>
   </x:si>
   <x:si>
     <x:t>haval128,4</x:t>
   </x:si>
   <x:si>
-    <x:t>31ba43a330bab68b3a974cfda488deca</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9ea4d153c9a5ff3d736b7e1018e0ddfc</x:t>
+    <x:t>fc86045e7238f0466ad44662bb86f987</x:t>
   </x:si>
   <x:si>
     <x:t>haval160,4</x:t>
   </x:si>
   <x:si>
-    <x:t>01883977856b4d1dae50002a53251715ed5ea42a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6242717bea5e9322934fd8e01bd8200ee3937190</x:t>
+    <x:t>a4efc2a92c046b344f9a5e73cfd6f86492770b5c</x:t>
   </x:si>
   <x:si>
     <x:t>haval192,4</x:t>
   </x:si>
   <x:si>
-    <x:t>b38c8dd023bc368183ce25912bec56dca48aab8b3faacdf3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>42c713aaa25e7dbd55b3480f97a95e0d35ea2df9c0bfac2c</x:t>
+    <x:t>f965b84a40c0f4af660918fcd088d5defe849cf7359b82eb</x:t>
   </x:si>
   <x:si>
     <x:t>haval224,4</x:t>
   </x:si>
   <x:si>
-    <x:t>8db87d9bbf8ebb73f8a961d7a5e66395f3651f6ebffae52b5269cc11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ce6dfe884d60a9933e8f5c894ba654399c31ad200c71d5a433a9b60d</x:t>
+    <x:t>f6d26fe7f470da9c803bd3888b96e1eb165fb82bfda4207d640ce4ee</x:t>
   </x:si>
   <x:si>
     <x:t>haval256,4</x:t>
   </x:si>
   <x:si>
-    <x:t>3c4e527a4448d75bb19ab5b7a3ad274a5cba0542400a70050e01535cb35a088e</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9ae9cab53c9168263645ec12978efbf040d181fc4a212aff0bd7787092aecb60</x:t>
+    <x:t>090bc3a2c1cf501784b6b2bdd81d872c52c146d27ecf45adef7246bec080c5bf</x:t>
   </x:si>
   <x:si>
     <x:t>haval128,5</x:t>
   </x:si>
   <x:si>
-    <x:t>ccce06ddd6e8ded1c7453cdbd512b333</x:t>
-  </x:si>
-  <x:si>
-    <x:t>496f76b5b462386c301f143f0c217818</x:t>
+    <x:t>c7cf0c1bbc8b60f4767668fb0ebb7b80</x:t>
   </x:si>
   <x:si>
     <x:t>haval160,5</x:t>
   </x:si>
   <x:si>
-    <x:t>64757d595cf621e89b66df489967c3e5433c5868</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0a41a208b6bba839cd7107e5bb92d025e1a5de3c</x:t>
+    <x:t>2252ad7ccbf0a54ceb21d7a8f275a489fed6f773</x:t>
   </x:si>
   <x:si>
     <x:t>haval192,5</x:t>
   </x:si>
   <x:si>
-    <x:t>9161a96775052e1696c555dd0be0db90381defcf2fa959b3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>acdacb89814f2b43d0e8b7fdeeecfd17aa04401be04c20bc</x:t>
+    <x:t>ff7744673ce7c4ed52db4e83be6d7969215077905c8b77f2</x:t>
   </x:si>
   <x:si>
     <x:t>haval224,5</x:t>
   </x:si>
   <x:si>
-    <x:t>c225a1f138be856a2a5d8c9ab2630f4a57d0b82c91c3177bdb0253e9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>93390b55c33fe279d0e3105084d2e9ffe8ae7a8018fb6371f4a28f2f</x:t>
+    <x:t>889d3c5bb93249de49ff3ee1d7b1d0ddf46d833fbe3a73fd8d01271b</x:t>
   </x:si>
   <x:si>
     <x:t>haval256,5</x:t>
   </x:si>
   <x:si>
-    <x:t>1a7cf5c88e84d2492077758389404e45acd142ffe87535d7204a7dabbd33273e</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7c0964233cbb9b0eb903e1b4a346f01cc4d825eae474f8d42d849ab8072d3fa8</x:t>
+    <x:t>e498784f5dda5d5ff23d1814df87a7a77b868d27d2549cbac21d728f31e7be38</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -244,9 +187,8 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -555,291 +497,236 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D20"/>
+  <x:dimension ref="A1:C20"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B2" sqref="B2 B2:B2"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
-    <x:col min="2" max="3" width="68.425781" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <x:col min="2" max="3" width="68.441406" style="1" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="2" t="s">
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="B2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="s">
+    </x:row>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="2" t="s">
+      <x:c r="B3" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="s">
+    </x:row>
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="B4" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="2" t="s">
+    </x:row>
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B4" s="2" t="s">
+      <x:c r="B5" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
+    </x:row>
+    <x:row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D4" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="2" t="s">
+      <x:c r="B6" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C6" s="1" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B5" s="2" t="s">
+    </x:row>
+    <x:row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A7" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+      <x:c r="B7" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C7" s="1" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D5" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="2" t="s">
+    </x:row>
+    <x:row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A8" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B6" s="2" t="s">
+      <x:c r="B8" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C8" s="1" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C6" s="2" t="s">
+    </x:row>
+    <x:row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A9" s="1" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D6" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="2" t="s">
+      <x:c r="B9" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C9" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B7" s="2" t="s">
+    </x:row>
+    <x:row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A10" s="1" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C7" s="2" t="s">
+      <x:c r="B10" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C10" s="1" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D7" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="2" t="s">
+    </x:row>
+    <x:row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A11" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B8" s="2" t="s">
+      <x:c r="B11" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C11" s="1" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C8" s="2" t="s">
+    </x:row>
+    <x:row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A12" s="1" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D8" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="2" t="s">
+      <x:c r="B12" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C12" s="1" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B9" s="2" t="s">
+    </x:row>
+    <x:row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A13" s="1" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C9" s="2" t="s">
+      <x:c r="B13" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C13" s="1" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D9" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="2" t="s">
+    </x:row>
+    <x:row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A14" s="1" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B10" s="2" t="s">
+      <x:c r="B14" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C14" s="1" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C10" s="2" t="s">
+    </x:row>
+    <x:row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A15" s="1" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D10" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="2" t="s">
+      <x:c r="B15" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C15" s="1" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B11" s="2" t="s">
+    </x:row>
+    <x:row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A16" s="1" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C11" s="2" t="s">
+      <x:c r="B16" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C16" s="1" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="D11" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="2" t="s">
+    </x:row>
+    <x:row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A17" s="1" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B12" s="2" t="s">
+      <x:c r="B17" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C17" s="1" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C12" s="2" t="s">
+    </x:row>
+    <x:row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A18" s="1" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D12" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="2" t="s">
+      <x:c r="B18" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C18" s="1" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B13" s="2" t="s">
+    </x:row>
+    <x:row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A19" s="1" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C13" s="2" t="s">
+      <x:c r="B19" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C19" s="1" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="D13" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="2" t="s">
+    </x:row>
+    <x:row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <x:c r="A20" s="1" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="B14" s="2" t="s">
+      <x:c r="B20" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C20" s="1" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="C14" s="2" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="D14" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="2" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="B15" s="2" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="C15" s="2" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="D15" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="2" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B16" s="2" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C16" s="2" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="D16" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="2" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="B17" s="2" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="C17" s="2" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D17" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="2" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B18" s="2" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C18" s="2" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="D18" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="2" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="B19" s="2" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="C19" s="2" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="D19" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="2" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="B20" s="2" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C20" s="2" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D20" s="2" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -852,15 +739,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Owner xmlns="5756a67b-a28b-4cf5-88e6-2b4468392c6e">
@@ -879,6 +757,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1113,20 +1000,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{597F7914-6EEE-4DD7-95D4-654EFC025ED0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B85D5699-EBE6-4BCF-8B5D-7A698D97386E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5756a67b-a28b-4cf5-88e6-2b4468392c6e"/>
     <ds:schemaRef ds:uri="2ace790c-9bff-4836-93d2-c906c881a70a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{597F7914-6EEE-4DD7-95D4-654EFC025ED0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>